<commit_message>
bug corrections after cold startup
</commit_message>
<xml_diff>
--- a/src/scripts/AUTOCONFIG.xlsx
+++ b/src/scripts/AUTOCONFIG.xlsx
@@ -5,7 +5,7 @@
   <fileSharing readOnlyRecommended="0" userName="nallin"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
+    <workbookView activeTab="1" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="102" sheetId="1" r:id="rId4"/>
@@ -14,17 +14,17 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1598036978" val="976" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1598036978" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1598036978" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1598036978"/>
+      <pm:revision xmlns:pm="smNativeData" day="1605106043" val="978" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1605106043" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1605106043" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1605106043"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="79">
   <si>
     <t>BBB_IP</t>
   </si>
@@ -221,28 +221,46 @@
     <t>10.128.103.104</t>
   </si>
   <si>
-    <t>BBB-PS-DCLink</t>
-  </si>
-  <si>
-    <t>FBP-DCLink</t>
+    <t>IA-03RaCtrl:CO-DCLinkCtrl</t>
+  </si>
+  <si>
+    <t>IA-03RaPS01:PS-DCLink-SI, IA-03RaPS02:PS-DCLink-SI</t>
+  </si>
+  <si>
+    <t>10.128.103.121</t>
+  </si>
+  <si>
+    <t>IA-03RaCtrl:CO-PSCtrl-SI1</t>
+  </si>
+  <si>
+    <t>SI-03M2:PS-QFP, SI-03M2:PS-QDP1, SI-03M2:PS-QDP2, SI-04M1:PS-QFB, SI-04M1:PS-QDB1, SI-04M1:PS-QDB2, SI-03M1:PS-QS, SI-03M2:PS-QS</t>
   </si>
   <si>
     <t>10.128.103.122</t>
   </si>
   <si>
-    <t>BBB-SI-CORRETORAS1</t>
-  </si>
-  <si>
-    <t>CH1,CH2,CV1,CV2,CH3,CH4,CV3</t>
+    <t>IA-03RaCtrl:CO-PSCtrl-SI2</t>
+  </si>
+  <si>
+    <t>SI-03M1:PS-CH, SI-03M1:PS-CV, SI-03M2:PS-CH, SI-03M2:PS-CV, SI-03C2:PS-CH, SI-03C2:PS-CV-1, SI-03C2:PS-CV-2</t>
+  </si>
+  <si>
+    <t>10.128.103.131</t>
+  </si>
+  <si>
+    <t>IA-03RaCtrl:CO-PSCtrl-SI3</t>
+  </si>
+  <si>
+    <t>SI-03C1:PS-Q1, SI-03C1:PS-Q2, SI-03C2:PS-Q3, SI-03C2:PS-Q4, SI-03C4:PS-Q1, SI-03C4:PS-Q2, SI-03C3:PS-Q3, SI-03C3:PS-Q4, SI-03C1:PS-QS, SI-03C2:PS-QS, SI-03C3:PS-QS</t>
   </si>
   <si>
     <t>10.128.103.132</t>
   </si>
   <si>
-    <t>BBB-SI-CORRETORAS2</t>
-  </si>
-  <si>
-    <t>CV4,CH5,CH6,CV5,CV6,CH7,CV7</t>
+    <t>IA-03RaCtrl:CO-PSCtrl-SI4</t>
+  </si>
+  <si>
+    <t>SI-03C1:PS-CH, SI-03C1:PS-CV, SI-03C4:PS-CH, SI-03C4:PS-CV, SI-03C3:PS-CH, SI-03C3:PS-CV-1, SI-03C3:PS-CV-2</t>
   </si>
 </sst>
 </file>
@@ -268,7 +286,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1598036978" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1605106043" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -283,7 +301,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1598036978" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1605106043" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -299,7 +317,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1598036978" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1605106043" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -321,7 +339,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1598036978" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1605106043" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -343,7 +361,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1598036978"/>
+          <pm:border xmlns:pm="smNativeData" id="1605106043"/>
         </ext>
       </extLst>
     </border>
@@ -362,7 +380,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1598036978"/>
+          <pm:border xmlns:pm="smNativeData" id="1605106043"/>
         </ext>
       </extLst>
     </border>
@@ -383,10 +401,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1598036978" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1605106043" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1598036978" count="5">
+      <pm:colors xmlns:pm="smNativeData" id="1605106043" count="5">
         <pm:color name="Color 24" rgb="95B3D7"/>
         <pm:color name="Color 25" rgb="DCE6F1"/>
         <pm:color name="Color 26" rgb="D8D8D8"/>
@@ -656,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="C1" zoomScale="175" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView view="normal" zoomScale="175" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -879,7 +897,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1598036978" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1605106043" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -888,14 +906,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1598036978" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1598036978" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1605106043" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1605106043" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1598036978" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1605106043" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -906,10 +924,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView view="normal" zoomScale="175" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" view="normal" zoomScale="175" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -1053,7 +1071,7 @@
         <v>27</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>69</v>
@@ -1074,13 +1092,47 @@
       </c>
       <c r="E10" s="1" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1598036978" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1605106043" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1089,14 +1141,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1598036978" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1598036978" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1605106043" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1605106043" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1598036978" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1605106043" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
organizing files and IA-04/05 added
</commit_message>
<xml_diff>
--- a/src/scripts/AUTOCONFIG.xlsx
+++ b/src/scripts/AUTOCONFIG.xlsx
@@ -10,21 +10,23 @@
   <sheets>
     <sheet name="102" sheetId="1" r:id="rId4"/>
     <sheet name="103" sheetId="2" r:id="rId5"/>
+    <sheet name="104" sheetId="3" r:id="rId6"/>
+    <sheet name="105" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1605106043" val="978" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1605106043" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1605106043" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1605106043"/>
+      <pm:revision xmlns:pm="smNativeData" day="1617130223" val="982" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1617130223" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1617130223" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1617130223"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="126">
   <si>
     <t>BBB_IP</t>
   </si>
@@ -261,6 +263,147 @@
   </si>
   <si>
     <t>SI-03C1:PS-CH, SI-03C1:PS-CV, SI-03C4:PS-CH, SI-03C4:PS-CV, SI-03C3:PS-CH, SI-03C3:PS-CV-1, SI-03C3:PS-CV-2</t>
+  </si>
+  <si>
+    <t>10.128.104.101</t>
+  </si>
+  <si>
+    <t>BBB-SALA04--VAC-MKS</t>
+  </si>
+  <si>
+    <t>10.128.104.102</t>
+  </si>
+  <si>
+    <t>BBB-SALA04-VAC-4UHV-BO-SI</t>
+  </si>
+  <si>
+    <t>11,12,13,14</t>
+  </si>
+  <si>
+    <t>10.128.104.117</t>
+  </si>
+  <si>
+    <t>BBB-SALA04-CON-MBTEMP-SR-BEFORE-BC</t>
+  </si>
+  <si>
+    <t>10.128.104.118</t>
+  </si>
+  <si>
+    <t>BBB-SALA04-CON-MBTEMP-SR-AFTER-BC</t>
+  </si>
+  <si>
+    <t>10.128.104.104</t>
+  </si>
+  <si>
+    <t>IA-04RaCtrl:CO-DCLinkCtrl</t>
+  </si>
+  <si>
+    <t>IA-04RaPS01:PS-DCLink-SI, IA-04RaPS02:PS-DCLink-SI</t>
+  </si>
+  <si>
+    <t>10.128.104.105</t>
+  </si>
+  <si>
+    <t>IA-04RaCtrl:CO-PSCtrl-BO</t>
+  </si>
+  <si>
+    <t>10.128.104.121</t>
+  </si>
+  <si>
+    <t>IA-04RaCtrl:CO-PSCtrl-SI1</t>
+  </si>
+  <si>
+    <t>10.128.104.122</t>
+  </si>
+  <si>
+    <t>IA-04RaCtrl:CO-PSCtrl-SI2</t>
+  </si>
+  <si>
+    <t>10.128.104.131</t>
+  </si>
+  <si>
+    <t>IA-04RaCtrl:CO-PSCtrl-SI3</t>
+  </si>
+  <si>
+    <t>10.128.104.132</t>
+  </si>
+  <si>
+    <t>IA-04RaCtrl:CO-PSCtrl-SI4</t>
+  </si>
+  <si>
+    <t>10.128.105.101</t>
+  </si>
+  <si>
+    <t>BBB-SALA05--VAC-MKS</t>
+  </si>
+  <si>
+    <t>10.128.105.102</t>
+  </si>
+  <si>
+    <t>BBB-SALA05-VAC-4UHV-BO</t>
+  </si>
+  <si>
+    <t>10.128.105.103</t>
+  </si>
+  <si>
+    <t>BBB-SALA05-VAC-4UHV-SI</t>
+  </si>
+  <si>
+    <t>10.128.105.106</t>
+  </si>
+  <si>
+    <t>BBB-SALA05-CON-MBTEMP-BO-06-10</t>
+  </si>
+  <si>
+    <t>10.128.105.117</t>
+  </si>
+  <si>
+    <t>BBB-SALA05-CON-MBTEMP-SR-BEFORE-BC</t>
+  </si>
+  <si>
+    <t>10.128.105.118</t>
+  </si>
+  <si>
+    <t>BBB-SALA05-CON-MBTEMP-SR-AFTER-BC</t>
+  </si>
+  <si>
+    <t>10.128.105.104</t>
+  </si>
+  <si>
+    <t>IA-05RaCtrl:CO-DCLinkCtrl</t>
+  </si>
+  <si>
+    <t>IA-05RaPS01:PS-DCLink-SI, IA-05RaPS02:PS-DCLink-SI</t>
+  </si>
+  <si>
+    <t>10.128.105.105</t>
+  </si>
+  <si>
+    <t>IA-05RaCtrl:CO-PSCtrl-BO</t>
+  </si>
+  <si>
+    <t>10.128.105.121</t>
+  </si>
+  <si>
+    <t>IA-05RaCtrl:CO-PSCtrl-SI1</t>
+  </si>
+  <si>
+    <t>10.128.105.122</t>
+  </si>
+  <si>
+    <t>IA-05RaCtrl:CO-PSCtrl-SI2</t>
+  </si>
+  <si>
+    <t>10.128.105.131</t>
+  </si>
+  <si>
+    <t>IA-05RaCtrl:CO-PSCtrl-SI3</t>
+  </si>
+  <si>
+    <t>10.128.105.132</t>
+  </si>
+  <si>
+    <t>IA-05RaCtrl:CO-PSCtrl-SI4</t>
   </si>
 </sst>
 </file>
@@ -286,7 +429,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1605106043" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1617130223" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -301,7 +444,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1605106043" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1617130223" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -317,7 +460,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1605106043" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1617130223" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -339,7 +482,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1605106043" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1617130223" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -361,7 +504,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1605106043"/>
+          <pm:border xmlns:pm="smNativeData" id="1617130223"/>
         </ext>
       </extLst>
     </border>
@@ -380,7 +523,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1605106043"/>
+          <pm:border xmlns:pm="smNativeData" id="1617130223"/>
         </ext>
       </extLst>
     </border>
@@ -401,10 +544,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1605106043" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1617130223" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1605106043" count="5">
+      <pm:colors xmlns:pm="smNativeData" id="1617130223" count="5">
         <pm:color name="Color 24" rgb="95B3D7"/>
         <pm:color name="Color 25" rgb="DCE6F1"/>
         <pm:color name="Color 26" rgb="D8D8D8"/>
@@ -675,7 +818,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView view="normal" zoomScale="175" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -897,7 +1040,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1605106043" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1617130223" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -906,14 +1049,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1605106043" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1605106043" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1617130223" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1617130223" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1605106043" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1617130223" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -935,6 +1078,241 @@
     <col min="1" max="1" width="15.774775" customWidth="1" style="1"/>
     <col min="2" max="2" width="38.702703" customWidth="1" style="1"/>
     <col min="3" max="3" width="15.765766" customWidth="1" style="1"/>
+    <col min="4" max="4" width="12.423423" customWidth="1" style="1"/>
+    <col min="5" max="5" width="29.558559" customWidth="1" style="1"/>
+    <col min="6" max="6" width="15.000000" customWidth="1" style="1"/>
+    <col min="7" max="16384" width="10.000000" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1617130223" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="1.000000" right="1.000000" top="1.000000" bottom="1.000000" header="0.393750" footer="0.393750"/>
+  <pageSetup paperSize="1" fitToWidth="0" fitToHeight="1" pageOrder="overThenDown"/>
+  <headerFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1617130223" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1617130223" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+      </ext>
+    </extLst>
+  </headerFooter>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1617130223" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView view="normal" zoomScale="175" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
+  <cols>
+    <col min="1" max="1" width="15.774775" customWidth="1" style="1"/>
+    <col min="2" max="2" width="38.702703" customWidth="1" style="1"/>
+    <col min="3" max="3" width="15.765766" customWidth="1" style="1"/>
     <col min="4" max="4" width="10.801802" customWidth="1" style="1"/>
     <col min="5" max="5" width="29.558559" customWidth="1" style="1"/>
     <col min="6" max="6" width="15.000000" customWidth="1" style="1"/>
@@ -961,10 +1339,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -975,164 +1353,126 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>53</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>28</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>67</v>
+        <v>95</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1605106043" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1617130223" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1141,14 +1481,239 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1605106043" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1605106043" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1617130223" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1617130223" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1605106043" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1617130223" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView view="normal" zoomScale="175" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
+  <cols>
+    <col min="1" max="1" width="15.774775" customWidth="1" style="1"/>
+    <col min="2" max="2" width="38.702703" customWidth="1" style="1"/>
+    <col min="3" max="3" width="15.765766" customWidth="1" style="1"/>
+    <col min="4" max="4" width="10.801802" customWidth="1" style="1"/>
+    <col min="5" max="5" width="51.693694" customWidth="1" style="1"/>
+    <col min="6" max="6" width="15.000000" customWidth="1" style="1"/>
+    <col min="7" max="16384" width="10.000000" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1617130223" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="1.000000" right="1.000000" top="1.000000" bottom="1.000000" header="0.393750" footer="0.393750"/>
+  <pageSetup paperSize="1" fitToWidth="0" fitToHeight="1" pageOrder="overThenDown"/>
+  <headerFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1617130223" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1617130223" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+      </ext>
+    </extLst>
+  </headerFooter>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1617130223" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Completing info about IA-04 and IA-05 BBBs
</commit_message>
<xml_diff>
--- a/src/scripts/AUTOCONFIG.xlsx
+++ b/src/scripts/AUTOCONFIG.xlsx
@@ -5,7 +5,7 @@
   <fileSharing readOnlyRecommended="0" userName="nallin"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
+    <workbookView activeTab="2" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="102" sheetId="1" r:id="rId4"/>
@@ -16,17 +16,17 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1617130223" val="982" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1617130223" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1617130223" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1617130223"/>
+      <pm:revision xmlns:pm="smNativeData" day="1617801532" val="982" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1617801532" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1617801532" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1617801532"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="136">
   <si>
     <t>BBB_IP</t>
   </si>
@@ -307,30 +307,45 @@
     <t>IA-04RaCtrl:CO-PSCtrl-BO</t>
   </si>
   <si>
+    <t>BO-07U:PS-CH, BO-07U:PS-CV, BO-09U:PS-CH, BO-09U:PS-CV</t>
+  </si>
+  <si>
     <t>10.128.104.121</t>
   </si>
   <si>
     <t>IA-04RaCtrl:CO-PSCtrl-SI1</t>
   </si>
   <si>
+    <t>SI-04M2:PS-QFB, SI-04M2:PS-QDB1, SI-04M2:PS-QDB2, SI-05M1:PS-QFA, SI-05M1:PS-QDA, SI-04M1:PS-QS, SI-04M2:PS-QS</t>
+  </si>
+  <si>
     <t>10.128.104.122</t>
   </si>
   <si>
     <t>IA-04RaCtrl:CO-PSCtrl-SI2</t>
   </si>
   <si>
+    <t>SI-04M1:PS-CH, SI-04M1:PS-CV, SI-04M2:PS-CH, SI-04M2:PS-CV, SI-04C2:PS-CH, SI-04C2:PS-CV-1, SI-04C2:PS-CV-2</t>
+  </si>
+  <si>
     <t>10.128.104.131</t>
   </si>
   <si>
     <t>IA-04RaCtrl:CO-PSCtrl-SI3</t>
   </si>
   <si>
+    <t>SI-04C1:PS-Q1, SI-04C1:PS-Q2, SI-04C2:PS-Q3, SI-04C2:PS-Q4, SI-04C4:PS-Q1, SI-04C4:PS-Q2, SI-04C3:PS-Q3, SI-04C3:PS-Q4, SI-04C1:PS-QS, SI-04C2:PS-QS, SI-04C3:PS-QS</t>
+  </si>
+  <si>
     <t>10.128.104.132</t>
   </si>
   <si>
     <t>IA-04RaCtrl:CO-PSCtrl-SI4</t>
   </si>
   <si>
+    <t>SI-04C1:PS-CH, SI-04C1:PS-CV, SI-04C4:PS-CH, SI-04C4:PS-CV, SI-04C3:PS-CH, SI-04C3:PS-CV-1, SI-04C3:PS-CV-2</t>
+  </si>
+  <si>
     <t>10.128.105.101</t>
   </si>
   <si>
@@ -382,28 +397,43 @@
     <t>IA-05RaCtrl:CO-PSCtrl-BO</t>
   </si>
   <si>
+    <t>BO-11U:PS-CH, BO-11U:PS-CV, BO-13U:PS-CH, BO-13U:PS-CV</t>
+  </si>
+  <si>
     <t>10.128.105.121</t>
   </si>
   <si>
     <t>IA-05RaCtrl:CO-PSCtrl-SI1</t>
   </si>
   <si>
+    <t>SI-05M2:PS-QFA, SI-05M2:PS-QDA, SI-06M1:PS-QFB, SI-06M1:PS-QDB1, SI-06M1:PS-QDB2, SI-05M1:PS-QS, SI-05M2:PS-QS</t>
+  </si>
+  <si>
     <t>10.128.105.122</t>
   </si>
   <si>
     <t>IA-05RaCtrl:CO-PSCtrl-SI2</t>
   </si>
   <si>
+    <t>SI-05M1:PS-CH, SI-05M1:PS-CV, SI-05M2:PS-CH, SI-05M2:PS-CV, SI-05C2:PS-CH, SI-05C2:PS-CV-1, SI-05C2:PS-CV-2</t>
+  </si>
+  <si>
     <t>10.128.105.131</t>
   </si>
   <si>
     <t>IA-05RaCtrl:CO-PSCtrl-SI3</t>
   </si>
   <si>
+    <t>SI-05C1:PS-Q1, SI-05C1:PS-Q2, SI-05C2:PS-Q3, SI-05C2:PS-Q4, SI-05C4:PS-Q1, SI-05C4:PS-Q2, SI-05C3:PS-Q3, SI-05C3:PS-Q4, SI-05C1:PS-QS, SI-05C2:PS-QS, SI-05C3:PS-QS</t>
+  </si>
+  <si>
     <t>10.128.105.132</t>
   </si>
   <si>
     <t>IA-05RaCtrl:CO-PSCtrl-SI4</t>
+  </si>
+  <si>
+    <t>SI-05C1:PS-CH, SI-05C1:PS-CV, SI-05C4:PS-CH, SI-05C4:PS-CV, SI-05C3:PS-CH, SI-05C3:PS-CV-1, SI-05C3:PS-CV-2</t>
   </si>
 </sst>
 </file>
@@ -429,7 +459,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1617130223" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1617801532" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -444,7 +474,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1617130223" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1617801532" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -460,7 +490,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1617130223" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1617801532" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -482,7 +512,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1617130223" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1617801532" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -504,7 +534,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1617130223"/>
+          <pm:border xmlns:pm="smNativeData" id="1617801532"/>
         </ext>
       </extLst>
     </border>
@@ -523,7 +553,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1617130223"/>
+          <pm:border xmlns:pm="smNativeData" id="1617801532"/>
         </ext>
       </extLst>
     </border>
@@ -544,10 +574,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1617130223" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1617801532" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1617130223" count="5">
+      <pm:colors xmlns:pm="smNativeData" id="1617801532" count="5">
         <pm:color name="Color 24" rgb="95B3D7"/>
         <pm:color name="Color 25" rgb="DCE6F1"/>
         <pm:color name="Color 26" rgb="D8D8D8"/>
@@ -1040,7 +1070,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1617130223" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1617801532" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1049,14 +1079,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1617130223" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1617130223" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1617801532" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1617801532" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1617130223" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1617801532" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1069,8 +1099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" zoomScale="175" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView view="normal" zoomScale="175" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -1275,7 +1305,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1617130223" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1617801532" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1284,14 +1314,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1617130223" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1617130223" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1617801532" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1617801532" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1617130223" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1617801532" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1304,8 +1334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView view="normal" zoomScale="175" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" view="normal" zoomScale="175" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -1423,56 +1453,83 @@
       <c r="D7" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E7" s="1" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1617130223" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1617801532" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1481,14 +1538,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1617130223" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1617130223" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1617801532" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1617801532" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1617130223" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1617801532" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1502,7 +1559,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView view="normal" zoomScale="175" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -1536,10 +1593,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -1550,10 +1607,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
@@ -1564,10 +1621,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -1578,10 +1635,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>18</v>
@@ -1592,10 +1649,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>18</v>
@@ -1606,10 +1663,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>18</v>
@@ -1620,10 +1677,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>27</v>
@@ -1632,15 +1689,15 @@
         <v>28</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>27</v>
@@ -1648,56 +1705,83 @@
       <c r="D9" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="E9" s="1" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>27</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1617130223" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1617801532" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1706,14 +1790,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1617130223" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1617130223" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1617801532" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1617801532" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1617130223" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1617801532" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
more bbbs in autoconfig
</commit_message>
<xml_diff>
--- a/src/scripts/AUTOCONFIG.xlsx
+++ b/src/scripts/AUTOCONFIG.xlsx
@@ -5,28 +5,31 @@
   <fileSharing readOnlyRecommended="0" userName="nallin"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="2" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
+    <workbookView activeTab="4" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="102" sheetId="1" r:id="rId4"/>
     <sheet name="103" sheetId="2" r:id="rId5"/>
     <sheet name="104" sheetId="3" r:id="rId6"/>
     <sheet name="105" sheetId="4" r:id="rId7"/>
+    <sheet name="106" sheetId="5" r:id="rId8"/>
+    <sheet name="107" sheetId="6" r:id="rId9"/>
+    <sheet name="108" sheetId="7" r:id="rId10"/>
   </sheets>
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1617801532" val="982" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1617801532" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1617801532" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1617801532"/>
+      <pm:revision xmlns:pm="smNativeData" day="1626094064" val="982" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1626094064" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1626094064" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1626094064"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="234">
   <si>
     <t>BBB_IP</t>
   </si>
@@ -175,6 +178,45 @@
     <t>SI-02C1:PS-CH, SI-02C1:PS-CV, SI-02C4:PS-CH, SI-02C4:PS-CV, SI-02C3:PS-CH, SI-02C3:PS-CV-1, SI-02C3:PS-CV-2</t>
   </si>
   <si>
+    <t>10.128.102.151</t>
+  </si>
+  <si>
+    <t>COUNTINGPRU-SI-02-M2</t>
+  </si>
+  <si>
+    <t>CountingPRU</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>10.128.102.152</t>
+  </si>
+  <si>
+    <t>COUNTINGPRU-SI-02-C2</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>10.128.102.153</t>
+  </si>
+  <si>
+    <t>COUNTINGPRU-SI-02-C3</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>10.128.102.154</t>
+  </si>
+  <si>
+    <t>COUNTINGPRU-SI-03-M1</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>10.128.103.101</t>
   </si>
   <si>
@@ -367,7 +409,7 @@
     <t>10.128.105.106</t>
   </si>
   <si>
-    <t>BBB-SALA05-CON-MBTEMP-BO-06-10</t>
+    <t>BBB-SALA05-CON-MBTEMP-BO-11-15</t>
   </si>
   <si>
     <t>10.128.105.117</t>
@@ -434,6 +476,261 @@
   </si>
   <si>
     <t>SI-05C1:PS-CH, SI-05C1:PS-CV, SI-05C4:PS-CH, SI-05C4:PS-CV, SI-05C3:PS-CH, SI-05C3:PS-CV-1, SI-05C3:PS-CV-2</t>
+  </si>
+  <si>
+    <t>10.128.106.101</t>
+  </si>
+  <si>
+    <t>BBB-SALA06--VAC-MKS</t>
+  </si>
+  <si>
+    <t>10.128.106.102</t>
+  </si>
+  <si>
+    <t>BBB-SALA06-VAC-4UHV-BO-SI</t>
+  </si>
+  <si>
+    <t>10.128.106.103</t>
+  </si>
+  <si>
+    <t>BBB-SALA06-VAC-4UHV-SI</t>
+  </si>
+  <si>
+    <t>10.128.106.117</t>
+  </si>
+  <si>
+    <t>BBB-SALA06-CON-MBTEMP-SR-BEFORE-BC</t>
+  </si>
+  <si>
+    <t>10.128.106.118</t>
+  </si>
+  <si>
+    <t>BBB-SALA06-CON-MBTEMP-SR-AFTER-BC</t>
+  </si>
+  <si>
+    <t>10.128.106.104</t>
+  </si>
+  <si>
+    <t>IA-06RaCtrl:CO-DCLinkCtrl</t>
+  </si>
+  <si>
+    <t>IA-06RaPS01:PS-DCLink-SI, IA-06RaPS02:PS-DCLink-SI</t>
+  </si>
+  <si>
+    <t>10.128.106.105</t>
+  </si>
+  <si>
+    <t>IA-06RaCtrl:CO-PSCtrl-BO</t>
+  </si>
+  <si>
+    <t>10.128.106.121</t>
+  </si>
+  <si>
+    <t>IA-06RaCtrl:CO-PSCtrl-SI1</t>
+  </si>
+  <si>
+    <t>SI-06M2:PS-QFB, SI-06M2:PS-QDB1, SI-06M2:PS-QDB2, SI-05M1:PS-QFA, SI-05M1:PS-QDA, SI-06M1:PS-QS, SI-06M2:PS-QS</t>
+  </si>
+  <si>
+    <t>10.128.106.122</t>
+  </si>
+  <si>
+    <t>IA-06RaCtrl:CO-PSCtrl-SI2</t>
+  </si>
+  <si>
+    <t>SI-06M1:PS-CH, SI-06M1:PS-CV, SI-06M2:PS-CH, SI-06M2:PS-CV, SI-06C2:PS-CH, SI-06C2:PS-CV-1, SI-06C2:PS-CV-2</t>
+  </si>
+  <si>
+    <t>10.128.106.131</t>
+  </si>
+  <si>
+    <t>IA-06RaCtrl:CO-PSCtrl-SI3</t>
+  </si>
+  <si>
+    <t>SI-06C1:PS-Q1, SI-06C1:PS-Q2, SI-06C2:PS-Q3, SI-06C2:PS-Q4, SI-06C4:PS-Q1, SI-06C4:PS-Q2, SI-06C3:PS-Q3, SI-06C3:PS-Q4, SI-06C1:PS-QS, SI-06C2:PS-QS, SI-06C3:PS-QS</t>
+  </si>
+  <si>
+    <t>10.128.106.132</t>
+  </si>
+  <si>
+    <t>IA-06RaCtrl:CO-PSCtrl-SI4</t>
+  </si>
+  <si>
+    <t>SI-06C1:PS-CH, SI-06C1:PS-CV, SI-06C4:PS-CH, SI-06C4:PS-CV, SI-06C3:PS-CH, SI-06C3:PS-CV-1, SI-06C3:PS-CV-2</t>
+  </si>
+  <si>
+    <t>10.128.107.101</t>
+  </si>
+  <si>
+    <t>BBB-SALA07--VAC-MKS</t>
+  </si>
+  <si>
+    <t>10.128.107.102</t>
+  </si>
+  <si>
+    <t>BBB-SALA07-VAC-4UHV-BO</t>
+  </si>
+  <si>
+    <t>10.128.107.103</t>
+  </si>
+  <si>
+    <t>BBB-SALA07-VAC-4UHV-SI</t>
+  </si>
+  <si>
+    <t>10.128.107.106</t>
+  </si>
+  <si>
+    <t>BBB-SALA07-CON-MBTEMP-BO-16-20</t>
+  </si>
+  <si>
+    <t>10.128.107.117</t>
+  </si>
+  <si>
+    <t>BBB-SALA07-CON-MBTEMP-SR-BEFORE-BC</t>
+  </si>
+  <si>
+    <t>10.128.107.118</t>
+  </si>
+  <si>
+    <t>BBB-SALA07-CON-MBTEMP-SR-AFTER-BC</t>
+  </si>
+  <si>
+    <t>10.128.107.104</t>
+  </si>
+  <si>
+    <t>IA-07RaCtrl:CO-DCLinkCtrl</t>
+  </si>
+  <si>
+    <t>IA-07RaPS01:PS-DCLink-SI, IA-07RaPS02:PS-DCLink-SI</t>
+  </si>
+  <si>
+    <t>10.128.107.105</t>
+  </si>
+  <si>
+    <t>IA-07RaCtrl:CO-PSCtrl-BO</t>
+  </si>
+  <si>
+    <t>BO-15U:PS-CH, BO-15U:PS-CV, BO-17U:PS-CH, BO-17U:PS-CV</t>
+  </si>
+  <si>
+    <t>10.128.107.121</t>
+  </si>
+  <si>
+    <t>IA-07RaCtrl:CO-PSCtrl-SI1</t>
+  </si>
+  <si>
+    <t>SI-07M2:PS-QFA, SI-07M2:PS-QDA, SI-06M1:PS-QFB, SI-06M1:PS-QDB1, SI-06M1:PS-QDB2, SI-07M1:PS-QS, SI-07M2:PS-QS</t>
+  </si>
+  <si>
+    <t>10.128.107.122</t>
+  </si>
+  <si>
+    <t>IA-07RaCtrl:CO-PSCtrl-SI2</t>
+  </si>
+  <si>
+    <t>SI-07M1:PS-CH, SI-07M1:PS-CV, SI-07M2:PS-CH, SI-07M2:PS-CV, SI-07C2:PS-CH, SI-07C2:PS-CV-1, SI-07C2:PS-CV-2</t>
+  </si>
+  <si>
+    <t>10.128.107.131</t>
+  </si>
+  <si>
+    <t>IA-07RaCtrl:CO-PSCtrl-SI3</t>
+  </si>
+  <si>
+    <t>SI-07C1:PS-Q1, SI-07C1:PS-Q2, SI-07C2:PS-Q3, SI-07C2:PS-Q4, SI-07C4:PS-Q1, SI-07C4:PS-Q2, SI-07C3:PS-Q3, SI-07C3:PS-Q4, SI-07C1:PS-QS, SI-07C2:PS-QS, SI-07C3:PS-QS</t>
+  </si>
+  <si>
+    <t>10.128.107.132</t>
+  </si>
+  <si>
+    <t>IA-07RaCtrl:CO-PSCtrl-SI4</t>
+  </si>
+  <si>
+    <t>SI-07C1:PS-CH, SI-07C1:PS-CV, SI-07C4:PS-CH, SI-07C4:PS-CV, SI-07C3:PS-CH, SI-07C3:PS-CV-1, SI-07C3:PS-CV-2</t>
+  </si>
+  <si>
+    <t>10.128.108.101</t>
+  </si>
+  <si>
+    <t>BBB-SALA08-VAC-MKS</t>
+  </si>
+  <si>
+    <t>10.128.108.102</t>
+  </si>
+  <si>
+    <t>BBB-SALA08-VAC-4UHV-BO-SI</t>
+  </si>
+  <si>
+    <t>10.128.108.103</t>
+  </si>
+  <si>
+    <t>BBB-SALA08-VAC-4UHV-SI</t>
+  </si>
+  <si>
+    <t>10.128.108.117</t>
+  </si>
+  <si>
+    <t>BBB-SALA08-CON-MBTEMP-SR-BEFORE-BC</t>
+  </si>
+  <si>
+    <t>10.128.108.118</t>
+  </si>
+  <si>
+    <t>BBB-SALA08-CON-MBTEMP-SR-AFTER-BC</t>
+  </si>
+  <si>
+    <t>10.128.108.104</t>
+  </si>
+  <si>
+    <t>IA-08RaCtrl:CO-DCLinkCtrl</t>
+  </si>
+  <si>
+    <t>IA-08RaPS01:PS-DCLink-SI, IA-08RaPS02:PS-DCLink-SI</t>
+  </si>
+  <si>
+    <t>10.128.108.105</t>
+  </si>
+  <si>
+    <t>IA-08RaCtrl:CO-PSCtrl-BO</t>
+  </si>
+  <si>
+    <t>BO-19U:PS-CH, BO-19U:PS-CV, BO-21U:PS-CH, BO-21U:PS-CV</t>
+  </si>
+  <si>
+    <t>10.128.108.121</t>
+  </si>
+  <si>
+    <t>IA-08RaCtrl:CO-PSCtrl-SI1</t>
+  </si>
+  <si>
+    <t>SI-08M2:PS-QFB, SI-08M2:PS-QDB1, SI-08M2:PS-QDB2, SI-05M1:PS-QFA, SI-05M1:PS-QDA, SI-08M1:PS-QS, SI-08M2:PS-QS</t>
+  </si>
+  <si>
+    <t>10.128.108.122</t>
+  </si>
+  <si>
+    <t>IA-08RaCtrl:CO-PSCtrl-SI2</t>
+  </si>
+  <si>
+    <t>SI-08M1:PS-CH, SI-08M1:PS-CV, SI-08M2:PS-CH, SI-08M2:PS-CV, SI-08C2:PS-CH, SI-08C2:PS-CV-1, SI-08C2:PS-CV-2</t>
+  </si>
+  <si>
+    <t>10.128.108.131</t>
+  </si>
+  <si>
+    <t>IA-08RaCtrl:CO-PSCtrl-SI3</t>
+  </si>
+  <si>
+    <t>SI-08C1:PS-Q1, SI-08C1:PS-Q2, SI-08C2:PS-Q3, SI-08C2:PS-Q4, SI-08C4:PS-Q1, SI-08C4:PS-Q2, SI-08C3:PS-Q3, SI-08C3:PS-Q4, SI-08C1:PS-QS, SI-08C2:PS-QS, SI-08C3:PS-QS</t>
+  </si>
+  <si>
+    <t>10.128.108.132</t>
+  </si>
+  <si>
+    <t>IA-08RaCtrl:CO-PSCtrl-SI4</t>
+  </si>
+  <si>
+    <t>SI-08C1:PS-CH, SI-08C1:PS-CV, SI-08C4:PS-CH, SI-08C4:PS-CV, SI-08C3:PS-CH, SI-08C3:PS-CV-1, SI-08C3:PS-CV-2</t>
   </si>
 </sst>
 </file>
@@ -451,7 +748,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _$_-;\-* #,##0.00\ _$_-;_-* &quot;-&quot;??\ _$_-;_-@_-"/>
     <numFmt numFmtId="49" formatCode="@"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Arial"/>
       <family val="2"/>
@@ -459,7 +756,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1617801532" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1626094064" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -474,7 +771,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1617801532" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1626094064" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -490,10 +787,25 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1617801532" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1626094064" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1626094064" ulstyle="none" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Basic Roman" sz="200" lang="default"/>
+            <pm:ea face="Basic Roman" sz="200" lang="default"/>
           </pm:charSpec>
         </ext>
       </extLst>
@@ -512,7 +824,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1617801532" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1626094064" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -534,7 +846,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1617801532"/>
+          <pm:border xmlns:pm="smNativeData" id="1626094064"/>
         </ext>
       </extLst>
     </border>
@@ -553,7 +865,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1617801532"/>
+          <pm:border xmlns:pm="smNativeData" id="1626094064"/>
         </ext>
       </extLst>
     </border>
@@ -561,12 +873,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -574,10 +887,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1617801532" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1626094064" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1617801532" count="5">
+      <pm:colors xmlns:pm="smNativeData" id="1626094064" count="5">
         <pm:color name="Color 24" rgb="95B3D7"/>
         <pm:color name="Color 25" rgb="DCE6F1"/>
         <pm:color name="Color 26" rgb="D8D8D8"/>
@@ -594,10 +907,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="D5D5D5"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="494949"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="EEECE1"/>
@@ -845,10 +1158,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView view="normal" zoomScale="175" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -1066,11 +1379,67 @@
         <v>48</v>
       </c>
     </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1617801532" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1626094064" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1079,14 +1448,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1617801532" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1617801532" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1626094064" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1626094064" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1617801532" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1626094064" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1134,10 +1503,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -1148,52 +1517,52 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>18</v>
@@ -1204,10 +1573,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>18</v>
@@ -1218,10 +1587,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>27</v>
@@ -1230,15 +1599,15 @@
         <v>28</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>27</v>
@@ -1247,15 +1616,15 @@
         <v>36</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>27</v>
@@ -1264,15 +1633,15 @@
         <v>40</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>27</v>
@@ -1281,15 +1650,15 @@
         <v>44</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>27</v>
@@ -1298,14 +1667,14 @@
         <v>40</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1617801532" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1626094064" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1314,14 +1683,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1617801532" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1617801532" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1626094064" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1626094064" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1617801532" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1626094064" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1334,7 +1703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" zoomScale="175" workbookViewId="0">
+    <sheetView view="normal" zoomScale="175" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -1369,10 +1738,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -1383,24 +1752,24 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>18</v>
@@ -1411,10 +1780,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>18</v>
@@ -1425,10 +1794,10 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>27</v>
@@ -1437,15 +1806,15 @@
         <v>28</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>27</v>
@@ -1454,15 +1823,15 @@
         <v>32</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>27</v>
@@ -1471,15 +1840,15 @@
         <v>40</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>27</v>
@@ -1488,15 +1857,15 @@
         <v>40</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>27</v>
@@ -1505,15 +1874,15 @@
         <v>44</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>27</v>
@@ -1522,14 +1891,14 @@
         <v>40</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1617801532" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1626094064" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1538,14 +1907,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1617801532" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1617801532" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1626094064" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1626094064" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1617801532" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1626094064" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1559,7 +1928,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView view="normal" zoomScale="175" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -1593,10 +1962,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -1607,52 +1976,52 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>18</v>
@@ -1663,10 +2032,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>18</v>
@@ -1677,10 +2046,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>27</v>
@@ -1689,15 +2058,15 @@
         <v>28</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>27</v>
@@ -1706,15 +2075,15 @@
         <v>32</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>27</v>
@@ -1723,15 +2092,15 @@
         <v>40</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>27</v>
@@ -1740,15 +2109,15 @@
         <v>40</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>27</v>
@@ -1757,15 +2126,15 @@
         <v>44</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>27</v>
@@ -1774,14 +2143,14 @@
         <v>40</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1617801532" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1626094064" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1790,14 +2159,742 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1617801532" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1617801532" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1626094064" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1626094064" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1617801532" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1626094064" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="normal" zoomScale="175" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
+  <cols>
+    <col min="1" max="1" width="15.774775" customWidth="1" style="1"/>
+    <col min="2" max="2" width="38.702703" customWidth="1" style="1"/>
+    <col min="3" max="3" width="15.765766" customWidth="1" style="1"/>
+    <col min="4" max="4" width="10.801802" customWidth="1" style="1"/>
+    <col min="5" max="5" width="29.558559" customWidth="1" style="1"/>
+    <col min="6" max="6" width="15.000000" customWidth="1" style="1"/>
+    <col min="7" max="16384" width="10.000000" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1626094064" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="1.000000" right="1.000000" top="1.000000" bottom="1.000000" header="0.393750" footer="0.393750"/>
+  <pageSetup paperSize="1" fitToWidth="0" fitToHeight="1" pageOrder="overThenDown"/>
+  <headerFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1626094064" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1626094064" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+      </ext>
+    </extLst>
+  </headerFooter>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1626094064" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView view="normal" zoomScale="175" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
+  <cols>
+    <col min="1" max="1" width="15.774775" customWidth="1" style="1"/>
+    <col min="2" max="2" width="38.702703" customWidth="1" style="1"/>
+    <col min="3" max="3" width="15.765766" customWidth="1" style="1"/>
+    <col min="4" max="4" width="10.801802" customWidth="1" style="1"/>
+    <col min="5" max="5" width="51.693694" customWidth="1" style="1"/>
+    <col min="6" max="6" width="15.000000" customWidth="1" style="1"/>
+    <col min="7" max="16384" width="10.000000" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1626094064" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="1.000000" right="1.000000" top="1.000000" bottom="1.000000" header="0.393750" footer="0.393750"/>
+  <pageSetup paperSize="1" fitToWidth="0" fitToHeight="1" pageOrder="overThenDown"/>
+  <headerFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1626094064" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1626094064" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+      </ext>
+    </extLst>
+  </headerFooter>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1626094064" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView view="normal" zoomScale="175" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
+  <cols>
+    <col min="1" max="1" width="15.774775" customWidth="1" style="1"/>
+    <col min="2" max="2" width="38.702703" customWidth="1" style="1"/>
+    <col min="3" max="3" width="15.765766" customWidth="1" style="1"/>
+    <col min="4" max="4" width="10.801802" customWidth="1" style="1"/>
+    <col min="5" max="5" width="29.558559" customWidth="1" style="1"/>
+    <col min="6" max="6" width="15.000000" customWidth="1" style="1"/>
+    <col min="7" max="16384" width="10.000000" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1626094064" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="1.000000" right="1.000000" top="1.000000" bottom="1.000000" header="0.393750" footer="0.393750"/>
+  <pageSetup paperSize="1" fitToWidth="0" fitToHeight="1" pageOrder="overThenDown"/>
+  <headerFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1626094064" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1626094064" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+      </ext>
+    </extLst>
+  </headerFooter>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1626094064" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>